<commit_message>
FrontEnd: DAC full Range und Status Register funktioniert
</commit_message>
<xml_diff>
--- a/MC_RthTEC_V0_0_5/COM_Protocol_V0_0_6.xlsx
+++ b/MC_RthTEC_V0_0_5/COM_Protocol_V0_0_6.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schmidm\Desktop\MC_RthTEC_Programm\MC_RthTEC_V_0_GIT\Protocol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schmidm\Desktop\MC_RthTEC_Programm\MC_RthTEC_V_0_GIT\MC_RthTEC_V0_0_5\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="134">
   <si>
     <t>Befehl</t>
   </si>
@@ -418,6 +418,39 @@
   </si>
   <si>
     <t>SWG[N]F = xW/O-Unit</t>
+  </si>
+  <si>
+    <t>SIN[N]F</t>
+  </si>
+  <si>
+    <t>Initialisierung für „FrontEnd“ Karte</t>
+  </si>
+  <si>
+    <t>GVF[N]F</t>
+  </si>
+  <si>
+    <t>Get Voltage full range (DAC 0 - 10V)</t>
+  </si>
+  <si>
+    <t>SWO = x mV</t>
+  </si>
+  <si>
+    <t>GVF[N]F=x mV</t>
+  </si>
+  <si>
+    <t>SWG[N]F = x W/O-Unit</t>
+  </si>
+  <si>
+    <t>SWO[N]F = x mV</t>
+  </si>
+  <si>
+    <t>GSI[N]F</t>
+  </si>
+  <si>
+    <t>Status Info (Range verlassen)</t>
+  </si>
+  <si>
+    <t>GVF[N]F=01010101</t>
   </si>
 </sst>
 </file>
@@ -597,7 +630,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -649,6 +682,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -951,10 +987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J42"/>
+  <dimension ref="B2:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,21 +1000,22 @@
     <col min="4" max="4" width="38.42578125" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="9" max="9" width="30.140625" customWidth="1"/>
+    <col min="11" max="11" width="43" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="H2" s="23" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="H2" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1008,17 +1045,17 @@
       </c>
     </row>
     <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="19"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="20"/>
       <c r="F5" s="3"/>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="19"/>
+      <c r="I5" s="20"/>
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1048,17 +1085,17 @@
       </c>
     </row>
     <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="19"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="20"/>
       <c r="F7" s="7"/>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="19"/>
+      <c r="I7" s="20"/>
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1160,17 +1197,17 @@
       </c>
     </row>
     <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="19"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="20"/>
       <c r="F12" s="7"/>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="19"/>
+      <c r="I12" s="20"/>
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="2:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1277,7 +1314,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>39</v>
       </c>
@@ -1303,21 +1340,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="18" t="s">
+    <row r="18" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="19"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="20"/>
       <c r="F18" s="8"/>
-      <c r="H18" s="18" t="s">
+      <c r="H18" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="I18" s="19"/>
+      <c r="I18" s="20"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="2:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="13" t="s">
         <v>43</v>
       </c>
@@ -1344,21 +1381,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="18" t="s">
+    <row r="20" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="19"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="20"/>
       <c r="F20" s="8"/>
-      <c r="H20" s="18" t="s">
+      <c r="H20" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="I20" s="19"/>
+      <c r="I20" s="20"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
         <v>47</v>
       </c>
@@ -1382,7 +1419,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="4" t="s">
         <v>50</v>
       </c>
@@ -1408,7 +1445,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
         <v>54</v>
       </c>
@@ -1434,21 +1471,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="18" t="s">
+    <row r="24" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="19"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="20"/>
       <c r="F24" s="9"/>
-      <c r="H24" s="18" t="s">
+      <c r="H24" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="I24" s="19"/>
+      <c r="I24" s="20"/>
       <c r="J24" s="9"/>
     </row>
-    <row r="25" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="4" t="s">
         <v>59</v>
       </c>
@@ -1470,7 +1507,7 @@
       </c>
       <c r="J25" s="10"/>
     </row>
-    <row r="26" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="4" t="s">
         <v>62</v>
       </c>
@@ -1492,7 +1529,7 @@
       </c>
       <c r="J26" s="10"/>
     </row>
-    <row r="27" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="4" t="s">
         <v>64</v>
       </c>
@@ -1514,307 +1551,371 @@
       </c>
       <c r="J27" s="10"/>
     </row>
-    <row r="28" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="18" t="s">
+    <row r="28" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="19"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="20"/>
       <c r="F28" s="9"/>
-      <c r="H28" s="18" t="s">
+      <c r="H28" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="I28" s="19"/>
+      <c r="I28" s="20"/>
       <c r="J28" s="9"/>
     </row>
-    <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F29" s="12" t="s">
         <v>109</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="I29" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="I29" s="5"/>
+      <c r="J29" s="12"/>
+    </row>
+    <row r="30" spans="2:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>121</v>
-      </c>
-      <c r="J29" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>122</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>109</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="J30" s="12" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="31" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="18" t="s">
+    <row r="31" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="J31" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="12"/>
+      <c r="H32" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="K32" s="18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="12"/>
+      <c r="H33" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="J33" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="K33" s="18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="9"/>
-      <c r="H31" s="18" t="s">
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="9"/>
+      <c r="H34" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="I31" s="19"/>
-      <c r="J31" s="9"/>
-    </row>
-    <row r="32" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="4" t="s">
+      <c r="I34" s="20"/>
+      <c r="J34" s="9"/>
+    </row>
+    <row r="35" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C35" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D35" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E35" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="F32" s="10"/>
-      <c r="H32" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J32" s="10"/>
-    </row>
-    <row r="33" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E33" s="5"/>
-      <c r="F33" s="10"/>
-      <c r="H33" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I33" s="5"/>
-      <c r="J33" s="10"/>
-    </row>
-    <row r="34" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="22"/>
-      <c r="H34" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I34" s="21"/>
-      <c r="J34" s="22"/>
-    </row>
-    <row r="35" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="F35" s="10"/>
       <c r="H35" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="J35" s="10"/>
+    </row>
+    <row r="36" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E36" s="5"/>
+      <c r="F36" s="10"/>
+      <c r="H36" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I36" s="5"/>
+      <c r="J36" s="10"/>
+    </row>
+    <row r="37" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="23"/>
+      <c r="H37" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="I37" s="22"/>
+      <c r="J37" s="23"/>
+    </row>
+    <row r="38" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="I35" s="5" t="s">
+      <c r="C38" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E38" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="J35" s="10"/>
-    </row>
-    <row r="36" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="4" t="s">
+      <c r="F38" s="10"/>
+      <c r="H38" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="J38" s="10"/>
+    </row>
+    <row r="39" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="J36" s="6"/>
-    </row>
-    <row r="37" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="J37" s="6"/>
-    </row>
-    <row r="38" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="J38" s="6"/>
-    </row>
-    <row r="39" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D39" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="J39" s="6"/>
+    </row>
+    <row r="40" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="J40" s="6"/>
+    </row>
+    <row r="41" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J41" s="6"/>
+    </row>
+    <row r="42" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="E42" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F39" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H39" s="4" t="s">
+      <c r="F42" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H42" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="I39" s="5" t="s">
+      <c r="I42" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="J39" s="6"/>
-    </row>
-    <row r="40" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="18" t="s">
+      <c r="J42" s="6"/>
+    </row>
+    <row r="43" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="9"/>
-      <c r="H40" s="18" t="s">
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="9"/>
+      <c r="H43" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="I40" s="19"/>
-      <c r="J40" s="9"/>
-    </row>
-    <row r="41" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="4" t="s">
+      <c r="I43" s="20"/>
+      <c r="J43" s="9"/>
+    </row>
+    <row r="44" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C44" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D44" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E44" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F41" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H41" s="4" t="s">
+      <c r="F44" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H44" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="I41" s="5" t="s">
+      <c r="I44" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="J41" s="6"/>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="11" t="s">
+      <c r="J44" s="6"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="11" t="s">
         <v>95</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
     <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B43:E43"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B28:E28"/>
@@ -1827,9 +1928,9 @@
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H34:J34"/>
-    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H37:J37"/>
+    <mergeCell ref="H43:I43"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="H28:I28"/>

</xml_diff>

<commit_message>
Reset FlipFlop auf FronEnd funktioniert
</commit_message>
<xml_diff>
--- a/MC_RthTEC_V0_0_5/COM_Protocol_V0_0_6.xlsx
+++ b/MC_RthTEC_V0_0_5/COM_Protocol_V0_0_6.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="137">
   <si>
     <t>Befehl</t>
   </si>
@@ -451,6 +451,15 @@
   </si>
   <si>
     <t>GVF[N]F=01010101</t>
+  </si>
+  <si>
+    <t>SRF[N]F</t>
+  </si>
+  <si>
+    <t>Keine</t>
+  </si>
+  <si>
+    <t>Reset FlipFlops</t>
   </si>
 </sst>
 </file>
@@ -689,6 +698,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -703,9 +715,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -987,10 +996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K45"/>
+  <dimension ref="B2:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,18 +1013,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="H2" s="24" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="H2" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1048,14 +1057,14 @@
       <c r="B5" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="21"/>
       <c r="F5" s="3"/>
       <c r="H5" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="20"/>
+      <c r="I5" s="21"/>
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1088,14 +1097,14 @@
       <c r="B7" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="21"/>
       <c r="F7" s="7"/>
       <c r="H7" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="20"/>
+      <c r="I7" s="21"/>
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1200,14 +1209,14 @@
       <c r="B12" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="7"/>
       <c r="H12" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="20"/>
+      <c r="I12" s="21"/>
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="2:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1314,7 +1323,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>39</v>
       </c>
@@ -1340,21 +1349,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
       <c r="F18" s="8"/>
       <c r="H18" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="I18" s="20"/>
+      <c r="I18" s="21"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="2:11" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="13" t="s">
         <v>43</v>
       </c>
@@ -1381,21 +1390,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="21"/>
       <c r="F20" s="8"/>
       <c r="H20" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="I20" s="20"/>
+      <c r="I20" s="21"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
         <v>47</v>
       </c>
@@ -1419,7 +1428,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="4" t="s">
         <v>50</v>
       </c>
@@ -1445,7 +1454,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
         <v>54</v>
       </c>
@@ -1471,21 +1480,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="21"/>
       <c r="F24" s="9"/>
       <c r="H24" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="I24" s="20"/>
+      <c r="I24" s="21"/>
       <c r="J24" s="9"/>
     </row>
-    <row r="25" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="4" t="s">
         <v>59</v>
       </c>
@@ -1507,7 +1516,7 @@
       </c>
       <c r="J25" s="10"/>
     </row>
-    <row r="26" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="4" t="s">
         <v>62</v>
       </c>
@@ -1529,7 +1538,7 @@
       </c>
       <c r="J26" s="10"/>
     </row>
-    <row r="27" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="4" t="s">
         <v>64</v>
       </c>
@@ -1551,21 +1560,21 @@
       </c>
       <c r="J27" s="10"/>
     </row>
-    <row r="28" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="21"/>
       <c r="F28" s="9"/>
       <c r="H28" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="I28" s="20"/>
+      <c r="I28" s="21"/>
       <c r="J28" s="9"/>
     </row>
-    <row r="29" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
         <v>123</v>
       </c>
@@ -1587,7 +1596,7 @@
       <c r="I29" s="5"/>
       <c r="J29" s="12"/>
     </row>
-    <row r="30" spans="2:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
         <v>116</v>
       </c>
@@ -1613,7 +1622,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="31" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="4" t="s">
         <v>118</v>
       </c>
@@ -1639,26 +1648,27 @@
         <v>109</v>
       </c>
     </row>
-    <row r="32" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="H32" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="12"/>
-      <c r="H32" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="I32" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="J32" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="K32" s="18" t="s">
-        <v>132</v>
-      </c>
+      <c r="I32" s="5"/>
+      <c r="J32" s="12"/>
     </row>
     <row r="33" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="4" t="s">
@@ -1669,256 +1679,277 @@
       <c r="E33" s="5"/>
       <c r="F33" s="12"/>
       <c r="H33" s="4" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="J33" s="12" t="s">
         <v>109</v>
       </c>
       <c r="K33" s="18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="12"/>
+      <c r="H34" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="J34" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="K34" s="18" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="34" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="19" t="s">
+    <row r="35" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="9"/>
-      <c r="H34" s="19" t="s">
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="9"/>
+      <c r="H35" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="I34" s="20"/>
-      <c r="J34" s="9"/>
-    </row>
-    <row r="35" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F35" s="10"/>
-      <c r="H35" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="J35" s="10"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="9"/>
     </row>
     <row r="36" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E36" s="5"/>
+        <v>71</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="F36" s="10"/>
       <c r="H36" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="J36" s="10"/>
+    </row>
+    <row r="37" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="I36" s="5"/>
-      <c r="J36" s="10"/>
-    </row>
-    <row r="37" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="21" t="s">
+      <c r="C37" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E37" s="5"/>
+      <c r="F37" s="10"/>
+      <c r="H37" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I37" s="5"/>
+      <c r="J37" s="10"/>
+    </row>
+    <row r="38" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="23"/>
-      <c r="H37" s="21" t="s">
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="24"/>
+      <c r="H38" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="I37" s="22"/>
-      <c r="J37" s="23"/>
-    </row>
-    <row r="38" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F38" s="10"/>
-      <c r="H38" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="J38" s="10"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="24"/>
     </row>
     <row r="39" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>10</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="F39" s="10"/>
       <c r="H39" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="J39" s="6"/>
+        <v>77</v>
+      </c>
+      <c r="J39" s="10"/>
     </row>
     <row r="40" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J40" s="6"/>
     </row>
     <row r="41" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D42" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J42" s="6"/>
+    </row>
+    <row r="43" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E43" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F42" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H42" s="4" t="s">
+      <c r="F43" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H43" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="I42" s="5" t="s">
+      <c r="I43" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="J42" s="6"/>
-    </row>
-    <row r="43" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="19" t="s">
+      <c r="J43" s="6"/>
+    </row>
+    <row r="44" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="9"/>
-      <c r="H43" s="19" t="s">
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="9"/>
+      <c r="H44" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="I43" s="20"/>
-      <c r="J43" s="9"/>
-    </row>
-    <row r="44" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="4" t="s">
+      <c r="I44" s="21"/>
+      <c r="J44" s="9"/>
+    </row>
+    <row r="45" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C45" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D45" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="E45" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F44" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H44" s="4" t="s">
+      <c r="F45" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H45" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="I44" s="5" t="s">
+      <c r="I45" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="J44" s="6"/>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B45" s="11" t="s">
+      <c r="J45" s="6"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="11" t="s">
         <v>95</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H38:J38"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H28:I28"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="H7:I7"/>
@@ -1927,13 +1958,13 @@
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B18:E18"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H37:J37"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B28:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
BreakDown Voltage Integration: Relais & V_DS (set)
</commit_message>
<xml_diff>
--- a/MC_RthTEC_V0_0_5/COM_Protocol_V0_0_6.xlsx
+++ b/MC_RthTEC_V0_0_5/COM_Protocol_V0_0_6.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="147">
   <si>
     <t>Befehl</t>
   </si>
@@ -461,11 +461,44 @@
   <si>
     <t>Reset FlipFlops</t>
   </si>
+  <si>
+    <t>SVG[N]B</t>
+  </si>
+  <si>
+    <t>"-20000 … 20000"</t>
+  </si>
+  <si>
+    <t>V_GS in mV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SVG[N]B= x.x V </t>
+  </si>
+  <si>
+    <t>GVG[N]B</t>
+  </si>
+  <si>
+    <t>GVD[N]B</t>
+  </si>
+  <si>
+    <t>GCD[N]B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GVG[N]B=x.x V </t>
+  </si>
+  <si>
+    <t>GVD[N]B=x.x V</t>
+  </si>
+  <si>
+    <t>GCD[N]B=x.x A</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="00000"/>
+  </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -639,7 +672,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -698,23 +731,26 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -996,10 +1032,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K46"/>
+  <dimension ref="B2:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,18 +1049,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="H2" s="25" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="H2" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1057,14 +1093,14 @@
       <c r="B5" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="21"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="20"/>
       <c r="F5" s="3"/>
       <c r="H5" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="21"/>
+      <c r="I5" s="20"/>
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1097,14 +1133,14 @@
       <c r="B7" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="21"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="20"/>
       <c r="F7" s="7"/>
       <c r="H7" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="21"/>
+      <c r="I7" s="20"/>
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1209,14 +1245,14 @@
       <c r="B12" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="21"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="20"/>
       <c r="F12" s="7"/>
       <c r="H12" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="21"/>
+      <c r="I12" s="20"/>
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="2:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1353,14 +1389,14 @@
       <c r="B18" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="21"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="20"/>
       <c r="F18" s="8"/>
       <c r="H18" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="I18" s="21"/>
+      <c r="I18" s="20"/>
       <c r="J18" s="8"/>
     </row>
     <row r="19" spans="2:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1394,14 +1430,14 @@
       <c r="B20" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="21"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="20"/>
       <c r="F20" s="8"/>
       <c r="H20" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="I20" s="21"/>
+      <c r="I20" s="20"/>
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1484,14 +1520,14 @@
       <c r="B24" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="21"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="20"/>
       <c r="F24" s="9"/>
       <c r="H24" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="I24" s="21"/>
+      <c r="I24" s="20"/>
       <c r="J24" s="9"/>
     </row>
     <row r="25" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1564,14 +1600,14 @@
       <c r="B28" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="21"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="20"/>
       <c r="F28" s="9"/>
       <c r="H28" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="I28" s="21"/>
+      <c r="I28" s="20"/>
       <c r="J28" s="9"/>
     </row>
     <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1716,14 +1752,14 @@
       <c r="B35" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="21"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="20"/>
       <c r="F35" s="9"/>
       <c r="H35" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="I35" s="21"/>
+      <c r="I35" s="20"/>
       <c r="J35" s="9"/>
     </row>
     <row r="36" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1767,18 +1803,18 @@
       <c r="J37" s="10"/>
     </row>
     <row r="38" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="23"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="24"/>
-      <c r="H38" s="22" t="s">
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="23"/>
+      <c r="H38" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="I38" s="23"/>
-      <c r="J38" s="24"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="23"/>
     </row>
     <row r="39" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="4" t="s">
@@ -1793,13 +1829,13 @@
       <c r="E39" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="F39" s="10"/>
+      <c r="F39" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="H39" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>77</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="I39" s="5"/>
       <c r="J39" s="10"/>
     </row>
     <row r="40" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1819,11 +1855,9 @@
         <v>10</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="I40" s="5" t="s">
-        <v>81</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="I40" s="5"/>
       <c r="J40" s="6"/>
     </row>
     <row r="41" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1843,11 +1877,9 @@
         <v>10</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="I41" s="5" t="s">
-        <v>84</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="I41" s="5"/>
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1867,11 +1899,9 @@
         <v>10</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="I42" s="5" t="s">
-        <v>87</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="I42" s="5"/>
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1891,65 +1921,121 @@
         <v>10</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="I43" s="5" t="s">
-        <v>90</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="I43" s="5"/>
       <c r="J43" s="6"/>
     </row>
     <row r="44" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="9"/>
-      <c r="H44" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="I44" s="21"/>
-      <c r="J44" s="9"/>
+      <c r="B44" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C44" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="J44" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="45" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="6"/>
+      <c r="H45" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="J45" s="6"/>
+    </row>
+    <row r="46" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46" s="26"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="6"/>
+      <c r="H46" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="J46" s="6"/>
+    </row>
+    <row r="47" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="9"/>
+      <c r="H47" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="I47" s="20"/>
+      <c r="J47" s="9"/>
+    </row>
+    <row r="48" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C48" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D48" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="E48" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F45" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H45" s="4" t="s">
+      <c r="F48" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H48" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="I45" s="5" t="s">
+      <c r="I48" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="J45" s="6"/>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B46" s="11" t="s">
+      <c r="J48" s="6"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="11" t="s">
         <v>95</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H38:J38"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B28:E28"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="H7:I7"/>
@@ -1958,13 +2044,13 @@
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H38:J38"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H28:I28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
V_DS und I_DS messung realisiert
</commit_message>
<xml_diff>
--- a/MC_RthTEC_V0_0_5/COM_Protocol_V0_0_6.xlsx
+++ b/MC_RthTEC_V0_0_5/COM_Protocol_V0_0_6.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="147">
   <si>
     <t>Befehl</t>
   </si>
@@ -728,9 +728,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -745,12 +751,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1035,7 +1035,7 @@
   <dimension ref="B2:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,18 +1049,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="H2" s="24" t="s">
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="H2" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1090,17 +1090,17 @@
       </c>
     </row>
     <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="22"/>
       <c r="F5" s="3"/>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="20"/>
+      <c r="I5" s="22"/>
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1130,17 +1130,17 @@
       </c>
     </row>
     <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="20"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="7"/>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="20"/>
+      <c r="I7" s="22"/>
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1242,17 +1242,17 @@
       </c>
     </row>
     <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="20"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="22"/>
       <c r="F12" s="7"/>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="20"/>
+      <c r="I12" s="22"/>
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="2:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1386,17 +1386,17 @@
       </c>
     </row>
     <row r="18" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="20"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="22"/>
       <c r="F18" s="8"/>
-      <c r="H18" s="19" t="s">
+      <c r="H18" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="I18" s="20"/>
+      <c r="I18" s="22"/>
       <c r="J18" s="8"/>
     </row>
     <row r="19" spans="2:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1427,17 +1427,17 @@
       </c>
     </row>
     <row r="20" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="20"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="22"/>
       <c r="F20" s="8"/>
-      <c r="H20" s="19" t="s">
+      <c r="H20" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="I20" s="20"/>
+      <c r="I20" s="22"/>
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1517,17 +1517,17 @@
       </c>
     </row>
     <row r="24" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="20"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="22"/>
       <c r="F24" s="9"/>
-      <c r="H24" s="19" t="s">
+      <c r="H24" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="I24" s="20"/>
+      <c r="I24" s="22"/>
       <c r="J24" s="9"/>
     </row>
     <row r="25" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1597,17 +1597,17 @@
       <c r="J27" s="10"/>
     </row>
     <row r="28" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="20"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="22"/>
       <c r="F28" s="9"/>
-      <c r="H28" s="19" t="s">
+      <c r="H28" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="I28" s="20"/>
+      <c r="I28" s="22"/>
       <c r="J28" s="9"/>
     </row>
     <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1749,17 +1749,17 @@
       </c>
     </row>
     <row r="35" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="20"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="22"/>
       <c r="F35" s="9"/>
-      <c r="H35" s="19" t="s">
+      <c r="H35" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="I35" s="20"/>
+      <c r="I35" s="22"/>
       <c r="J35" s="9"/>
     </row>
     <row r="36" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1803,18 +1803,18 @@
       <c r="J37" s="10"/>
     </row>
     <row r="38" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="23"/>
-      <c r="H38" s="21" t="s">
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="25"/>
+      <c r="H38" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="I38" s="22"/>
-      <c r="J38" s="23"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="25"/>
     </row>
     <row r="39" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="4" t="s">
@@ -1930,7 +1930,7 @@
       <c r="B44" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C44" s="26" t="s">
+      <c r="C44" s="19" t="s">
         <v>138</v>
       </c>
       <c r="D44" s="5" t="s">
@@ -1966,13 +1966,15 @@
       <c r="I45" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="J45" s="6"/>
+      <c r="J45" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="46" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C46" s="26"/>
+      <c r="C46" s="19"/>
       <c r="D46" s="5"/>
       <c r="E46" s="4"/>
       <c r="F46" s="6"/>
@@ -1982,20 +1984,22 @@
       <c r="I46" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="J46" s="6"/>
+      <c r="J46" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="47" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="19" t="s">
+      <c r="B47" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="20"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="22"/>
       <c r="F47" s="9"/>
-      <c r="H47" s="19" t="s">
+      <c r="H47" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="I47" s="20"/>
+      <c r="I47" s="22"/>
       <c r="J47" s="9"/>
     </row>
     <row r="48" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2029,13 +2033,13 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H38:J38"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H28:I28"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="H7:I7"/>
@@ -2044,13 +2048,13 @@
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B18:E18"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H38:J38"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B28:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>